<commit_message>
Laboratorio 4 - Entrega Final
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4.xlsx
+++ b/Docs/Tablas Lab 4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michellevargas/Desktop/LABORATORIO S4/LabSorts-S04-G12/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E197636-5D23-49AC-AB0F-C814FF421F77}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{308F6AA6-9F08-A84D-AC70-7B128489C0C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="9140" yWindow="3620" windowWidth="18060" windowHeight="15580" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <r>
       <t>T</t>
@@ -79,12 +79,93 @@
       <t>amaño de la muestra (ARRAYLIST)</t>
     </r>
   </si>
+  <si>
+    <t>1204.77</t>
+  </si>
+  <si>
+    <t>97.89</t>
+  </si>
+  <si>
+    <t>4301.4</t>
+  </si>
+  <si>
+    <t>5166.38</t>
+  </si>
+  <si>
+    <t>145.0</t>
+  </si>
+  <si>
+    <t>18100.2</t>
+  </si>
+  <si>
+    <t>21852.62</t>
+  </si>
+  <si>
+    <t>273.63</t>
+  </si>
+  <si>
+    <t>68046.01</t>
+  </si>
+  <si>
+    <t>87621.64</t>
+  </si>
+  <si>
+    <t>751.72</t>
+  </si>
+  <si>
+    <t>276567.76</t>
+  </si>
+  <si>
+    <t>345676.9</t>
+  </si>
+  <si>
+    <t>1677.47</t>
+  </si>
+  <si>
+    <t>1219690.03</t>
+  </si>
+  <si>
+    <t>1345281.62</t>
+  </si>
+  <si>
+    <t>4074.0</t>
+  </si>
+  <si>
+    <t>10434.87</t>
+  </si>
+  <si>
+    <t>22171.97</t>
+  </si>
+  <si>
+    <t>74850.68</t>
+  </si>
+  <si>
+    <t>65228.5</t>
+  </si>
+  <si>
+    <t>636187.64</t>
+  </si>
+  <si>
+    <t>562823.63</t>
+  </si>
+  <si>
+    <t>3964.07</t>
+  </si>
+  <si>
+    <t>18131.16</t>
+  </si>
+  <si>
+    <t>83405.33</t>
+  </si>
+  <si>
+    <t>452448.8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +230,81 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -312,81 +468,6 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -459,7 +540,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -526,7 +607,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -613,17 +694,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -650,48 +731,33 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
+              <c:f>'Datos Lab4'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -741,57 +807,12 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -818,48 +839,33 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
+              <c:f>'Datos Lab4'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -867,7 +873,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EA19-4908-9336-CD0E2C6ECFDA}"/>
+              <c16:uniqueId val="{00000006-0324-1949-9D69-A384480FB39F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -909,56 +915,12 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -985,48 +947,42 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
+              <c:f>'Datos Lab4'!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1034,7 +990,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-EA19-4908-9336-CD0E2C6ECFDA}"/>
+              <c16:uniqueId val="{00000007-0324-1949-9D69-A384480FB39F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1126,7 +1082,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1164,7 +1120,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1248,7 +1204,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1286,7 +1242,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1328,7 +1284,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1365,7 +1321,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1374,7 +1330,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1441,7 +1397,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1456,7 +1412,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$B$14</c:f>
+              <c:f>'Datos Lab4'!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1528,17 +1484,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$14:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1565,48 +1521,21 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
+              <c:f>'Datos Lab4'!$B$14:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1623,7 +1552,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$C$14</c:f>
+              <c:f>'Datos Lab4'!$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1696,85 +1625,36 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
-              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+            <c:strRef>
+              <c:f>'Datos Lab4'!$C$14:$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>65228.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>562823.63</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
+              <c:f>'Datos Lab4'!$C$14:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1791,7 +1671,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$D$14</c:f>
+              <c:f>'Datos Lab4'!$D$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1863,17 +1743,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$14:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1900,48 +1780,27 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
+              <c:f>'Datos Lab4'!$D$14:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2041,7 +1900,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2079,7 +1938,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -2163,7 +2022,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2201,7 +2060,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -2243,7 +2102,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2280,7 +2139,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2289,7 +2148,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2356,7 +2215,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2444,17 +2303,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2481,48 +2340,33 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
+              <c:f>'Datos Lab4'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2539,7 +2383,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$B$14</c:f>
+              <c:f>'Datos Lab4'!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2612,17 +2456,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$14:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2649,48 +2493,21 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
+              <c:f>'Datos Lab4'!$B$14:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2790,7 +2607,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2828,7 +2645,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2907,7 +2724,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2945,7 +2762,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2987,7 +2804,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3024,7 +2841,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3033,7 +2850,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3095,7 +2912,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3183,17 +3000,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3220,48 +3037,33 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
+              <c:f>'Datos Lab4'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3278,7 +3080,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$C$14</c:f>
+              <c:f>'Datos Lab4'!$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3351,17 +3153,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$14:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3388,48 +3190,21 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
+              <c:f>'Datos Lab4'!$C$14:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3529,7 +3304,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3567,7 +3342,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3646,7 +3421,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3684,7 +3459,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3726,7 +3501,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3763,7 +3538,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3772,7 +3547,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3834,7 +3609,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3922,17 +3697,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3959,48 +3734,42 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
+              <c:f>'Datos Lab4'!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4017,7 +3786,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$D$14</c:f>
+              <c:f>'Datos Lab4'!$D$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4090,17 +3859,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$14:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4127,48 +3896,27 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
+              <c:f>'Datos Lab4'!$D$14:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4268,7 +4016,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4306,7 +4054,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4385,7 +4133,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4423,7 +4171,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4465,7 +4213,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4502,7 +4250,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -7286,7 +7034,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="135" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7297,7 +7045,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="135" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7308,7 +7056,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="135" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7330,7 +7078,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="135" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7341,7 +7089,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8683037" cy="6293556"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7374,7 +7122,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="8683037" cy="6293556"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7407,7 +7155,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="8683037" cy="6293556"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7473,7 +7221,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8685893" cy="6293304"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7503,33 +7251,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A13:D22" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A13:D22" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:D24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A14:D24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:D10" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7825,21 +7573,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="139" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7853,333 +7601,221 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="16">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
+        <v>1108</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
       </c>
-      <c r="D2" s="4">
-        <v>4</v>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="16">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
-      <c r="B3" s="4">
-        <v>20</v>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
       </c>
-      <c r="C3" s="4">
-        <v>2</v>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
       </c>
-      <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="16">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
-      <c r="B4" s="4">
-        <v>30</v>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
       </c>
-      <c r="C4" s="4">
-        <f>C3+C2</f>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16">
+      <c r="A5" s="1">
+        <v>8000</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16">
+      <c r="A6" s="1">
+        <v>16000</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="1">
+        <v>32000</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" s="1">
+        <v>64000</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16">
+      <c r="A9" s="1">
+        <v>128000</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>256000</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4">
+        <v>375942</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
+    </row>
+    <row r="14" spans="1:4" ht="16">
+      <c r="A14" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16">
+      <c r="A15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A5" s="1">
+    <row r="16" spans="1:4" ht="16">
+      <c r="A16" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16">
+      <c r="A17" s="1">
         <v>8000</v>
       </c>
-      <c r="B5" s="4">
-        <v>40</v>
-      </c>
-      <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
-      </c>
-      <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A6" s="1">
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
         <v>16000</v>
       </c>
-      <c r="B6" s="4">
-        <v>50</v>
-      </c>
-      <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A7" s="1">
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
         <v>32000</v>
       </c>
-      <c r="B7" s="4">
-        <v>60</v>
-      </c>
-      <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A8" s="1">
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
         <v>64000</v>
       </c>
-      <c r="B8" s="4">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A9" s="1">
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
         <v>128000</v>
       </c>
-      <c r="B9" s="4">
-        <v>80</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A10" s="1">
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
         <v>256000</v>
       </c>
-      <c r="B10" s="4">
-        <v>90</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A11" s="1">
-        <v>512000</v>
-      </c>
-      <c r="B11" s="4">
-        <v>100</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A15" s="1">
-        <v>1000</v>
-      </c>
-      <c r="B15" s="4">
-        <v>50</v>
-      </c>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A16" s="1">
-        <v>2000</v>
-      </c>
-      <c r="B16" s="4">
-        <v>60</v>
-      </c>
-      <c r="C16" s="4">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4">
-        <f>D15+43</f>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A17" s="1">
-        <v>4000</v>
-      </c>
-      <c r="B17" s="4">
-        <v>70</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
-      </c>
-      <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A18" s="1">
-        <v>8000</v>
-      </c>
-      <c r="B18" s="4">
-        <v>80</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="D18" s="4">
-        <f t="shared" si="3"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A19" s="1">
-        <v>16000</v>
-      </c>
-      <c r="B19" s="4">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="D19" s="4">
-        <f t="shared" si="3"/>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A20" s="1">
-        <v>32000</v>
-      </c>
-      <c r="B20" s="4">
-        <v>100</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A21" s="1">
-        <v>64000</v>
-      </c>
-      <c r="B21" s="4">
-        <v>110</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="3"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A22" s="1">
-        <v>128000</v>
-      </c>
-      <c r="B22" s="4">
-        <v>120</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="3"/>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A23" s="1">
-        <v>256000</v>
-      </c>
-      <c r="B23" s="4">
-        <v>130</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="3"/>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A24" s="1">
-        <v>512000</v>
-      </c>
-      <c r="B24" s="4">
-        <v>140</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="2"/>
-        <v>178</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>158</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8191,12 +7827,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8411,15 +8044,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8444,10 +8081,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>